<commit_message>
update templates to new miappe ontology version
</commit_message>
<xml_diff>
--- a/background information/GEO/GEO_mapping.xlsx
+++ b/background information/GEO/GEO_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stella Eggels\sciebo - Eggels, Stella (s.eggels@fz-juelich.de)@fz-juelich.sciebo.de\SE\DataPLANT\Metadata meetings\SWATE templates meetings\Repository requirements etc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stella Eggels\Documents\GitHub\Swate-templates\background information\GEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDBCB537-3FD0-4526-A7AC-699B14DC22AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855EFF90-89E2-406E-ADF2-EF05AC412521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{60BFCAF7-F63D-4737-85E9-88D1E08102D0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{60BFCAF7-F63D-4737-85E9-88D1E08102D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -74,9 +74,6 @@
     <t>title</t>
   </si>
   <si>
-    <t>Sample ID</t>
-  </si>
-  <si>
     <t>Assay</t>
   </si>
   <si>
@@ -144,6 +141,9 @@
   </si>
   <si>
     <t>**one of these is required &gt; just keep tissue because most relevant to plants</t>
+  </si>
+  <si>
+    <t>Sample description</t>
   </si>
 </sst>
 </file>
@@ -548,19 +548,20 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -568,10 +569,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -590,10 +591,10 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -604,37 +605,37 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -645,18 +646,18 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -664,68 +665,68 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12" s="1"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
         <v>21</v>
       </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
         <v>24</v>
       </c>
-      <c r="B16" t="s">
-        <v>25</v>
-      </c>
       <c r="C16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
         <v>27</v>
       </c>
-      <c r="B18" t="s">
-        <v>28</v>
-      </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -733,21 +734,21 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>